<commit_message>
cambios en clase agenda y galeria
se cambio la relacion de galeria con compendio y se agrego un atributo de estado en agenda
</commit_message>
<xml_diff>
--- a/Fichas Casos de Uso Tecnico.xlsx
+++ b/Fichas Casos de Uso Tecnico.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E54E4BE-231F-465B-AAAE-2C78FEE3E37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7297A1C5-01A2-4854-933A-CFA27FCFA87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
   </bookViews>
@@ -317,6 +317,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -335,20 +338,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F274FABB-DF5C-4F9E-B98F-F8DC866DADF5}">
   <dimension ref="B2:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,49 +681,49 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="3" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="15"/>
     </row>
     <row r="4" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="6" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="13"/>
     </row>
     <row r="7" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -734,7 +734,7 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="4">
         <v>1</v>
       </c>
@@ -743,7 +743,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="4">
         <v>2</v>
       </c>
@@ -752,7 +752,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="4">
         <v>3</v>
       </c>
@@ -761,19 +761,19 @@
       </c>
     </row>
     <row r="11" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
     </row>
@@ -781,56 +781,56 @@
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="19"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="14"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="14"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="14"/>
+      <c r="D19" s="15"/>
     </row>
     <row r="20" spans="2:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="12"/>
+      <c r="D20" s="13"/>
     </row>
     <row r="21" spans="2:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="12"/>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -841,7 +841,7 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="4">
         <v>1</v>
       </c>
@@ -850,7 +850,7 @@
       </c>
     </row>
     <row r="24" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="4">
         <v>2</v>
       </c>
@@ -859,7 +859,7 @@
       </c>
     </row>
     <row r="25" spans="2:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="4">
         <v>3</v>
       </c>
@@ -868,7 +868,7 @@
       </c>
     </row>
     <row r="26" spans="2:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="4">
         <v>4</v>
       </c>
@@ -877,21 +877,21 @@
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="4">
         <v>5</v>
       </c>
       <c r="D27" s="5"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="4">
         <v>6</v>
       </c>
       <c r="D28" s="5"/>
     </row>
     <row r="29" spans="2:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -901,8 +901,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
+    <row r="30" spans="2:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="10"/>
       <c r="C30" s="4" t="s">
         <v>24</v>
       </c>
@@ -911,7 +911,7 @@
       </c>
     </row>
     <row r="31" spans="2:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="4" t="s">
         <v>25</v>
       </c>
@@ -920,30 +920,30 @@
       </c>
     </row>
     <row r="32" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="9"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="4"/>
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="4"/>
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="4"/>
       <c r="D34" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="12"/>
+      <c r="D35" s="13"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
@@ -954,49 +954,49 @@
       <c r="B38" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="14"/>
+      <c r="D38" s="15"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="14"/>
+      <c r="D39" s="15"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="14"/>
+      <c r="D40" s="15"/>
     </row>
     <row r="41" spans="2:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="12"/>
+      <c r="D41" s="13"/>
     </row>
     <row r="42" spans="2:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="12"/>
+      <c r="D42" s="13"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -1007,7 +1007,7 @@
       </c>
     </row>
     <row r="44" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" s="9"/>
+      <c r="B44" s="10"/>
       <c r="C44" s="4">
         <v>1</v>
       </c>
@@ -1016,7 +1016,7 @@
       </c>
     </row>
     <row r="45" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B45" s="9"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="4">
         <v>2</v>
       </c>
@@ -1025,7 +1025,7 @@
       </c>
     </row>
     <row r="46" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B46" s="9"/>
+      <c r="B46" s="10"/>
       <c r="C46" s="4">
         <v>3</v>
       </c>
@@ -1034,7 +1034,7 @@
       </c>
     </row>
     <row r="47" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B47" s="9"/>
+      <c r="B47" s="10"/>
       <c r="C47" s="4">
         <v>4</v>
       </c>
@@ -1043,7 +1043,7 @@
       </c>
     </row>
     <row r="48" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="9"/>
+      <c r="B48" s="10"/>
       <c r="C48" s="4">
         <v>5</v>
       </c>
@@ -1052,7 +1052,7 @@
       </c>
     </row>
     <row r="49" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B49" s="10"/>
+      <c r="B49" s="11"/>
       <c r="C49" s="4">
         <v>6</v>
       </c>
@@ -1061,7 +1061,7 @@
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="4" t="s">
@@ -1070,45 +1070,61 @@
       <c r="D50" s="5"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="9"/>
+      <c r="B51" s="10"/>
       <c r="C51" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D51" s="5"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="9"/>
+      <c r="B52" s="10"/>
       <c r="C52" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D52" s="5"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="9"/>
+      <c r="B53" s="10"/>
       <c r="C53" s="4"/>
       <c r="D53" s="5"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="9"/>
+      <c r="B54" s="10"/>
       <c r="C54" s="4"/>
       <c r="D54" s="5"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="10"/>
+      <c r="B55" s="11"/>
       <c r="C55" s="4"/>
       <c r="D55" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="56" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="19" t="s">
+      <c r="B56" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="11"/>
-      <c r="D56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="B43:B49"/>
     <mergeCell ref="B50:B55"/>
     <mergeCell ref="C56:D56"/>
@@ -1117,22 +1133,6 @@
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>